<commit_message>
Email functionality and page structure
</commit_message>
<xml_diff>
--- a/scrapy/static/data/buildings+in+Thane+Ad+Advertiser.xlsx
+++ b/scrapy/static/data/buildings+in+Thane+Ad+Advertiser.xlsx
@@ -454,15 +454,16 @@
       <c r="A2" t="inlineStr">
         <is>
           <t>Sponsored
-Launching 2 BHK in Thane West | 40+ Indoor &amp; Outdoor Amenities
-raymondtenxera.com
-https://www.raymondtenxera.com › thane › project
-New Launch Homes by Raymond with 38 Habitable Floors, 26500 SqFt Clubhouse, 40+ Amenities</t>
+2 BHK Projects in Thane West | Starts at ₹93 Lacs* by Runwal
+landsend.runwal.com
+http://landsend.runwal.com › projects › thane
+Take Advantage of the Umbrella Offer: 2 BHK Flats Starts at ₹93L* at Lands End by Runwal. Book Your Dream Home at Runwal Lands End And Avail Pay 10% Now &amp; 90% On...
+View Location · View Gallery · Lands End by Runwal · Project Overview · Project Highlights</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Raymond Limited</t>
+          <t>Realatte Ventures LLP</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -475,15 +476,15 @@
       <c r="A3" t="inlineStr">
         <is>
           <t>Sponsored
-Tata Serein Phase II in Thane West, Thane - Price
-Housing
-https://www.housing.com
-3 BHK Apartments in Thane West | Luxurious Apartments in Thane | Prices Starting @ 2.75cr</t>
+1,2,3 BHK by Lodha® in Thane - 1 BHK by Lodha® in Thane
+Lodha Group
+https://www.lodhagroup.in
+World-class 1 BHKs in Thane by India's #1 real estate developer. Building a better life.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Locon Solutions Pvt. Ltd.</t>
+          <t>Macrotech Developers Limited</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -496,17 +497,16 @@
       <c r="A4" t="inlineStr">
         <is>
           <t>Sponsored
-2 BHK Projects in Thane West | Starts at ₹93 Lacs* by Runwal
-landsend.runwal.com
-http://landsend.runwal.com › projects › thane
-Take Advantage of the Umbrella Offer: 2 BHK Flats Starts at ₹93L* at Lands End by Runwal. Book Your Dream Home at Runwal Lands End And Avail Pay 10% Now &amp; 90% On Possession Plan. Kendriya Vidyalaya :2Mins.
-View Location · View Gallery · Lands End by Runwal · Location Advantages
-Call us</t>
+Godrej Exquisite, Thane | The Best of Thane
+Godrej Properties
+https://www.godrejproperties.com
+No shared walls between homes | Dual-lobby offers enhanced privacy | Grand Clubhouse. 2&amp;3 BHK Homes starting from ₹1.59 Cr* With Zero Stamp Duty &amp; Registration* Skyscape Gym. Dual-Lobby System. Rooftop Jacuzzi &amp; Spa.
+Location Details · Property Overview · Podium Amenities · Contact Us · Exclusive Amenities</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Realatte Ventures LLP</t>
+          <t>Madison Communications Private Limited</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">

</xml_diff>

<commit_message>
Structure of page, Login Signup functionalities
</commit_message>
<xml_diff>
--- a/scrapy/static/data/buildings+in+Thane+Ad+Advertiser.xlsx
+++ b/scrapy/static/data/buildings+in+Thane+Ad+Advertiser.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,37 +454,37 @@
       <c r="A2" t="inlineStr">
         <is>
           <t>Sponsored
+Launching 2 BHK in Thane West - Pay 20% &amp; Nothing till Jan'25
+raymondtenxera.com
+https://www.raymondtenxera.com › thane › project
+Experience a futuristic lifestyle with Raymond Realty's Spacious 2 BHK homes in Thane West. Prime Connectivity: School - 5 Mins | Metro - 3 Mins | Hospital - 2 Mins | Mall - 2 Mins.</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Raymond Limited</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sponsored
 2 BHK Projects in Thane West | Starts at ₹93 Lacs* by Runwal
 landsend.runwal.com
 http://landsend.runwal.com › projects › thane
-Take Advantage of the Umbrella Offer: 2 BHK Flats Starts at ₹93L* at Lands End by Runwal. Book Your Dream Home at Runwal Lands End And Avail Pay 10% Now &amp; 90% On...
-View Location · View Gallery · Lands End by Runwal · Project Overview · Project Highlights</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
+Take Advantage of the Umbrella Offer: 2 BHK Flats Starts at ₹93L* at Lands End by Runwal. Book Your Dream Home at Runwal Lands End And Avail Pay 10% Now &amp; 90% On Possession Plan. Kendriya Vidyalaya :2Mins. Amenities: Mini Theatre, Putting Golf.
+View Location · View Gallery · View Configurations · Project Configuration · Project Overview</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Realatte Ventures LLP</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Sponsored
-1,2,3 BHK by Lodha® in Thane - 1 BHK by Lodha® in Thane
-Lodha Group
-https://www.lodhagroup.in
-World-class 1 BHKs in Thane by India's #1 real estate developer. Building a better life.</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Macrotech Developers Limited</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -497,10 +497,10 @@
       <c r="A4" t="inlineStr">
         <is>
           <t>Sponsored
-Godrej Exquisite, Thane | The Best of Thane
+2&amp;3 BHK Homes at ₹1.59 Cr+* | The Best of Thane
 Godrej Properties
-https://www.godrejproperties.com
-No shared walls between homes | Dual-lobby offers enhanced privacy | Grand Clubhouse. 2&amp;3 BHK Homes starting from ₹1.59 Cr* With Zero Stamp Duty &amp; Registration* Skyscape Gym. Dual-Lobby System. Rooftop Jacuzzi &amp; Spa.
+https://www.godrejproperties.com › godrej
+Skyscape Gym — No shared walls between homes | Dual-lobby offers enhanced privacy | Grand Clubhouse. 2&amp;3 BHK Homes starting from ₹1.59 Cr* With Zero Stamp Duty &amp; Registration* Dual-Lobby System.
 Location Details · Property Overview · Podium Amenities · Contact Us · Exclusive Amenities</t>
         </is>
       </c>
@@ -510,6 +510,27 @@
         </is>
       </c>
       <c r="C4" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sponsored
+2 &amp; 3 BHK Homes at Thane - At Balkum, Thane (W)
+dostiwillow.com
+https://www.dostiwillow.com › homes › thane
+Dosti Willow at Thane | Project by Dosti™ Realty | Thane's Signature Living Expanded</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>DOSTI REALTY LIMITED</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>India</t>
         </is>

</xml_diff>